<commit_message>
bitacoras 1 2 3
</commit_message>
<xml_diff>
--- a/Bitacioras/bitacoras antiguas/01 Bitacora - jhoan sebastian blanco cataño/[respaldo] 01 Bitacora - jhoan sebastian blanco cataño.xlsx
+++ b/Bitacioras/bitacoras antiguas/01 Bitacora - jhoan sebastian blanco cataño/[respaldo] 01 Bitacora - jhoan sebastian blanco cataño.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\bitacoras antiguas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA CAT\Desktop\Blog-del-centro-agroturistico-SENA\Bitacioras\bitacoras antiguas\01 Bitacora - jhoan sebastian blanco cataño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4061FFD-43F8-467F-9182-C0E6141005A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED443848-7762-4947-9EF4-A19A4BF89550}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16755" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="220">
   <si>
     <t>Código: 
 GFPI-F-147</t>
@@ -841,81 +841,10 @@
     <t>X</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>DOCUMENTO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Avances del blog.docx]</t>
-    </r>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
     <t>sin dificultades</t>
-  </si>
-  <si>
-    <t>nuevo widget, es una imagen que estaba en el anterior blog del sena, solo que busque a fuente original y esta tiene mejor resolucion, ademas la comprimi para que ocupara menos
-comenxe a a subir css de los widgets a rruba, asi tener el css en un mismo lugar adema que ahia carga mas rapido que abajo
-cree un boton para desplegar el menu cuando este se plega, estube probando varios diseños y ese fue el que mas me gusto
-quise no agregar solo ese boton si no que agregar un menu de navegacion que sirva tanto para subir y bajar del todo de la pagina
-esto por que frankling lo tomo como un problema por que la pagina es muy larga</t>
-  </si>
-  <si>
-    <t>al seleccionar una un link del menu lateral este ahora se vulve verde y se desplaza a la derecha con un pequeño efectode rebote (la idea de esto vino un movimiento que hacia en el blog anterior)
-mejore las animaciones al saltar, cuando se pone el mause sobre una la animacion de salto anterior se desactiva y antes se sumaba
-agrege el efecto rebote a los botones de menu superior, inferior y a los botones sociales del blog ademas tambien fue agregado a las imagenes</t>
-  </si>
-  <si>
-    <t>el menu se expanidia mucho en la vercion de pc, le puse im limite 320px
-la fecha tiene animacion de oprimirse, los siguientes elementos transforman el cursor en la manita señalando: fechas, redes sociales
-puse el css del carusel de imagenes y los de paginacion en la secion &lt;b:template-skin&gt; ahora al recargar la pagina no se ve el bug en el que la imagen se volvia muy agrande unos segundos
-añadi mas botones al menu flotante, home, avanzar pagina, retroceder pagina, el boton de scrolear asia abajo fue modificado, su funcion ahora es compartida con la misma que maneja el scroll al oprimir una fecha. antes el scroll lleva hasta donde el main se terminaba, ahora se alcanza a ver un poco el futer</t>
-  </si>
-  <si>
-    <t>me dividi un poco en cosas nuevas por implementar, primero un foto de perfil con tu nombre de google, tambien traje de nuevo la barra de busque de blogger donde trae las cosas de cambiar de cambie el color de los botones de navegacion a verde, al estar inavilitados ya no tienen fondo como antes, en el codigo le puse clases mas cortas "menu-inferior-navegacion-btn" -&gt; "blog-navegacion" para agregarle el "-disable " al final
-removi el menu antiguo, pensaba dejarlo pero me parecia inesesario ya que esas opciones ya estan en el menu flotante</t>
-  </si>
-  <si>
-    <t>en la mañana estuve en una sita siquiatrica y parte de la tarde tuvimos que formarnos para raclamar los medicamentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">segui acomodando las paginas del blog
-mejore la documentacion para customizar el menu principal, y crear carpetas en este ultimo
-habia un bug que no permitia crear las carpetas con espasios, esto debido a que las IDs no se formaban bien, identifique el problema y removi los espacios al crear y buscar IDs
-ahora cuando se agrega un link que se abrira en otra pestaña a una imagen, esta ya no tienen el boton de descarga ni tampoco si puede oprimir para averla en el listado, le agrege mas cambios al final, solo admite si es una imagen que viene de blogger, si tiene un link basio esta si inavilita </t>
-  </si>
-  <si>
-    <t>ahora cuando una imagen tiene una url invalidad o no tienen url aparece un mensaje de error
-reorganize de mejor forma la pagina de politica ambiental de siga
-agregle un bug que hacia que aveces una pagina de desplazara a la derecha
-le propuse a mi profesor dos propuestas de diseños al poner imagenes en el menu, luego le di unos retoques a la que eliguio y cree una funcion que hace que al oprimir el link de una imagen del menu derecho se habra en una nueva pestaña, esto ya que desde blogger no se podia hacer antes</t>
-  </si>
-  <si>
-    <t>estava enseñandole algunas funciones del blog a frankling, cuando aparecio un error cuando varias imagenes estaban dentro de un h2, luego de esto decidi mover la forma de posicionamiento de las publicaciones (algo que no hacia hace mucho tiempo) afortunadamente ahora conosco  mucho mejor el blog y no me tomo tanto tiempo como antes
-ahora hay una forma de organizar que traera menos errores a la hora de hacer una publicacion, igual estuve atento a cualquier error que pudiera sugir, afortunamente los que sugieron los remedie rapidamente 
-las animaciones de los iframes has sido removidad, estas se veian exesivas y sobraban en los videos o pdfs
-ahora al asignar como titulo un elemento en blogger, este se colorea como el color primario de la pagina, esto es bastante util para poner el color de manera mas rapida, esto lo agrege a la documentacion
-agrege el grupo de servicios y agrege todas la paginas</t>
   </si>
   <si>
     <t xml:space="preserve">Desde 19/12/2024 hasta 2/01/2024 </t>
@@ -946,6 +875,46 @@
       </rPr>
       <t>[Avances.docx]</t>
     </r>
+  </si>
+  <si>
+    <t>comencé a desarrollarlo en Figma, una herramienta de maquetado muy completa. Aprendí lo esencial de ella, como guardar variables o definir temas de colores para facilitar su reasignación.
+Además, aprendí muchas otras cosas que desconocía del programa y todo lo que podía implementar en el proyecto, como el uso de componentes, lo cual permite una mayor escalabilidad.</t>
+  </si>
+  <si>
+    <t>Comencé a recibir pago el 21 de diciembre (sábado), por lo que inicié mi primera actividad el día 23. Edgar Mauricio empezó a explicarme lo que debía elaborar.
+Tenía que maquetar un software cuya finalidad era mejorar la administración del inventario en el SENA. Luego de explicarme lo básico, comenze a dibujar las conseptos basicos de la interfas en un papel demas de anotar la informacion relevante que debia mostrar el programa</t>
+  </si>
+  <si>
+    <t>Restablecimiento de contraseña: Acompañando el login, creé las ventanas para restablecer la contraseña, utilizando el método clásico de enviar un enlace de recuperación por correo electrónico.</t>
+  </si>
+  <si>
+    <t>Página principal: Diseñé la página principal, donde se visualizarían los productos. Coloqué secciones en la parte superior y un botón para cambiar entre modos de visualización. Agregué también una barra de búsqueda con una opción de filtros, los cuales se organizan en la parte inferior.</t>
+  </si>
+  <si>
+    <t>Productos de ejemplo: Se puede ver toda la información relevante de un producto ingresado al sistema, junto a un símbolo representativo.
+Menú desplegable: En la esquina superior izquierda, diseñé un menú desplegable que por ahora muestra únicamente la información de la cuenta del usuario, además de opciones para editar el perfil y cerrar sesión.</t>
+  </si>
+  <si>
+    <t>Filtro de búsqueda: Un diseño simple que permite seleccionar los filtros que se desean aplicar a una búsqueda. Se puede filtrar por tipo, unidad, categoría, subcategoría y fecha de ingreso al sistema. También hay una opción para ver únicamente los productos a cargo del usuario.</t>
+  </si>
+  <si>
+    <t>Componentes: Aunque no forman parte del diseño visual, son fundamentales para la escalabilidad del proyecto. A través de ellos se pueden modificar elementos globalmente en toda la página, lo que permite implementar cambios de forma rápida y eficiente.</t>
+  </si>
+  <si>
+    <t>Colores: Al igual que los componentes, forman parte del sistema de diseño. Creé una zona donde están definidos todos los colores utilizados, y empleé variables al asignarlos en la página. Esto permite cambiar un color en toda la interfaz fácilmente y mantener un orden visual, al trabajar con una paleta limitada de opciones.</t>
+  </si>
+  <si>
+    <t>La modalidad fue híbrida, ya que la mayor parte del maquetado la hice desde casa, con reuniones semanales para supervisar mi avance y despejar mis dudas, debido a que no había un software ni documentos hechos en los cuales pudiera apoyarme.</t>
+  </si>
+  <si>
+    <t>Sinceramente, se sentía raro estar maquetando esto sin siquiera un documento formal con los requerimientos funcionales y no funcionales; era como construir el techo de una casa sin tener aún las paredes.</t>
+  </si>
+  <si>
+    <t>Diseño del login: Comencé diseñando la pantalla de inicio de sesión para la plataforma. Utilicé como colores principales el blanco y el verde, ya que son representativos del SENA. Adicionalmente a esto inclui logos de este mismo
+estuve un buen rato experimentando con el fondo hasta que me decidi por dejarlo hasi con un aspecto difuminado</t>
+  </si>
+  <si>
+    <t>no habia empezado aun con mis funciones laborales</t>
   </si>
 </sst>
 </file>
@@ -4778,8 +4747,8 @@
   </sheetPr>
   <dimension ref="B1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5272,7 +5241,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="224" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G17" s="225"/>
       <c r="H17" s="20"/>
@@ -5951,7 +5920,7 @@
       <c r="X39" s="18"/>
       <c r="Y39" s="18"/>
     </row>
-    <row r="40" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:26" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="216"/>
       <c r="C40" s="217"/>
       <c r="D40" s="161">
@@ -5961,7 +5930,9 @@
         <v>45645</v>
       </c>
       <c r="F40" s="160"/>
-      <c r="G40" s="160"/>
+      <c r="G40" s="160" t="s">
+        <v>219</v>
+      </c>
       <c r="H40" s="20"/>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
@@ -5981,7 +5952,7 @@
       <c r="X40" s="18"/>
       <c r="Y40" s="18"/>
     </row>
-    <row r="41" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:26" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="216"/>
       <c r="C41" s="217"/>
       <c r="D41" s="161">
@@ -5991,7 +5962,9 @@
         <v>45646</v>
       </c>
       <c r="F41" s="160"/>
-      <c r="G41" s="160"/>
+      <c r="G41" s="160" t="s">
+        <v>219</v>
+      </c>
       <c r="H41" s="20"/>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
@@ -6063,9 +6036,9 @@
       <c r="X43" s="18"/>
       <c r="Y43" s="18"/>
     </row>
-    <row r="44" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:26" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="216" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C44" s="217"/>
       <c r="D44" s="161">
@@ -6075,10 +6048,10 @@
         <v>45649</v>
       </c>
       <c r="F44" s="160" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="160" t="s">
         <v>216</v>
-      </c>
-      <c r="G44" s="160" t="s">
-        <v>206</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="18"/>
@@ -6099,13 +6072,23 @@
       <c r="X44" s="18"/>
       <c r="Y44" s="18"/>
     </row>
-    <row r="45" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="216"/>
+    <row r="45" spans="2:26" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="216" t="s">
+        <v>208</v>
+      </c>
       <c r="C45" s="217"/>
-      <c r="D45" s="161"/>
-      <c r="E45" s="161"/>
-      <c r="F45" s="160"/>
-      <c r="G45" s="160"/>
+      <c r="D45" s="161">
+        <v>45650</v>
+      </c>
+      <c r="E45" s="161">
+        <v>45650</v>
+      </c>
+      <c r="F45" s="160" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="160" t="s">
+        <v>217</v>
+      </c>
       <c r="H45" s="20"/>
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
@@ -6125,13 +6108,23 @@
       <c r="X45" s="18"/>
       <c r="Y45" s="18"/>
     </row>
-    <row r="46" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="216"/>
+    <row r="46" spans="2:26" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="216" t="s">
+        <v>218</v>
+      </c>
       <c r="C46" s="217"/>
-      <c r="D46" s="161"/>
-      <c r="E46" s="161"/>
-      <c r="F46" s="160"/>
-      <c r="G46" s="160"/>
+      <c r="D46" s="161">
+        <v>45651</v>
+      </c>
+      <c r="E46" s="161">
+        <v>45651</v>
+      </c>
+      <c r="F46" s="160" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46" s="160" t="s">
+        <v>205</v>
+      </c>
       <c r="H46" s="20"/>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
@@ -6151,22 +6144,22 @@
       <c r="X46" s="18"/>
       <c r="Y46" s="18"/>
     </row>
-    <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:26" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="216" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C47" s="217"/>
       <c r="D47" s="161">
-        <v>45786</v>
+        <v>45652</v>
       </c>
       <c r="E47" s="161">
-        <v>45786</v>
+        <v>45652</v>
       </c>
       <c r="F47" s="160" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G47" s="160" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="18"/>
@@ -6187,22 +6180,22 @@
       <c r="X47" s="18"/>
       <c r="Y47" s="18"/>
     </row>
-    <row r="48" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:26" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="216" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C48" s="217"/>
       <c r="D48" s="161">
-        <v>45787</v>
+        <v>45653</v>
       </c>
       <c r="E48" s="161">
-        <v>45787</v>
+        <v>45653</v>
       </c>
       <c r="F48" s="160" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>
@@ -6224,22 +6217,12 @@
       <c r="Y48" s="18"/>
     </row>
     <row r="49" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="216" t="s">
-        <v>207</v>
-      </c>
+      <c r="B49" s="216"/>
       <c r="C49" s="217"/>
-      <c r="D49" s="161">
-        <v>45804</v>
-      </c>
-      <c r="E49" s="161">
-        <v>45804</v>
-      </c>
-      <c r="F49" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G49" s="160" t="s">
-        <v>206</v>
-      </c>
+      <c r="D49" s="161"/>
+      <c r="E49" s="161"/>
+      <c r="F49" s="160"/>
+      <c r="G49" s="160"/>
       <c r="H49" s="20"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
@@ -6260,22 +6243,12 @@
       <c r="Y49" s="18"/>
     </row>
     <row r="50" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="216" t="s">
-        <v>208</v>
-      </c>
+      <c r="B50" s="216"/>
       <c r="C50" s="217"/>
-      <c r="D50" s="161">
-        <v>45805</v>
-      </c>
-      <c r="E50" s="161">
-        <v>45805</v>
-      </c>
-      <c r="F50" s="160" t="s">
-        <v>204</v>
-      </c>
-      <c r="G50" s="160" t="s">
-        <v>206</v>
-      </c>
+      <c r="D50" s="161"/>
+      <c r="E50" s="161"/>
+      <c r="F50" s="160"/>
+      <c r="G50" s="160"/>
       <c r="H50" s="20"/>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
@@ -6295,22 +6268,22 @@
       <c r="X50" s="18"/>
       <c r="Y50" s="18"/>
     </row>
-    <row r="51" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:26" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="216" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C51" s="217"/>
       <c r="D51" s="161">
-        <v>45806</v>
+        <v>45656</v>
       </c>
       <c r="E51" s="161">
-        <v>45806</v>
+        <v>45656</v>
       </c>
       <c r="F51" s="160" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G51" s="160" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H51" s="20"/>
       <c r="I51" s="18"/>
@@ -6331,22 +6304,22 @@
       <c r="X51" s="18"/>
       <c r="Y51" s="18"/>
     </row>
-    <row r="52" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:26" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="216" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C52" s="217"/>
       <c r="D52" s="161">
-        <v>45807</v>
+        <v>45657</v>
       </c>
       <c r="E52" s="161">
-        <v>45807</v>
+        <v>45657</v>
       </c>
       <c r="F52" s="160" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G52" s="160" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="18"/>
@@ -6367,13 +6340,23 @@
       <c r="X52" s="18"/>
       <c r="Y52" s="18"/>
     </row>
-    <row r="53" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="216"/>
+    <row r="53" spans="2:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="216" t="s">
+        <v>214</v>
+      </c>
       <c r="C53" s="217"/>
-      <c r="D53" s="161"/>
-      <c r="E53" s="161"/>
-      <c r="F53" s="160"/>
-      <c r="G53" s="160"/>
+      <c r="D53" s="161">
+        <v>45658</v>
+      </c>
+      <c r="E53" s="161">
+        <v>45658</v>
+      </c>
+      <c r="F53" s="160" t="s">
+        <v>207</v>
+      </c>
+      <c r="G53" s="160" t="s">
+        <v>205</v>
+      </c>
       <c r="H53" s="20"/>
       <c r="I53" s="18"/>
       <c r="J53" s="18"/>
@@ -6393,13 +6376,23 @@
       <c r="X53" s="18"/>
       <c r="Y53" s="18"/>
     </row>
-    <row r="54" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="216"/>
+    <row r="54" spans="2:26" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="216" t="s">
+        <v>215</v>
+      </c>
       <c r="C54" s="217"/>
-      <c r="D54" s="161"/>
-      <c r="E54" s="161"/>
-      <c r="F54" s="160"/>
-      <c r="G54" s="160"/>
+      <c r="D54" s="161">
+        <v>45659</v>
+      </c>
+      <c r="E54" s="161">
+        <v>45659</v>
+      </c>
+      <c r="F54" s="160" t="s">
+        <v>207</v>
+      </c>
+      <c r="G54" s="160" t="s">
+        <v>205</v>
+      </c>
       <c r="H54" s="20"/>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
@@ -6655,7 +6648,7 @@
     </row>
     <row r="63" spans="2:26" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="97" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C63" s="98">
         <v>1</v>

</xml_diff>